<commit_message>
add chi-yun in observer list
</commit_message>
<xml_diff>
--- a/observations/TOP_ObservationLog.xlsx
+++ b/observations/TOP_ObservationLog.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E161"/>
+  <dimension ref="A1:E169"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1111,7 +1111,7 @@
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>WASP-90b</t>
+          <t>Qatar-1b</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
@@ -1131,14 +1131,14 @@
       </c>
       <c r="E26" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/WASP-90b_2192_2023-07-06_Altair1999_1323_Lum</t>
+          <t>https://www.exoclock.space/database/observations/Qatar-1b_6047_2023-07-06_Altair1999_1323_Lum</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Qatar-1b</t>
+          <t>WASP-90b</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -1158,7 +1158,7 @@
       </c>
       <c r="E27" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/Qatar-1b_6047_2023-07-06_Altair1999_1323_Lum</t>
+          <t>https://www.exoclock.space/database/observations/WASP-90b_2192_2023-07-06_Altair1999_1323_Lum</t>
         </is>
       </c>
     </row>
@@ -1516,7 +1516,7 @@
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>TOI-2154b</t>
+          <t>EPIC246851721b</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -1531,19 +1531,19 @@
       </c>
       <c r="D41" t="inlineStr">
         <is>
-          <t>NTHU Observatory</t>
+          <t>NTHU TAT</t>
         </is>
       </c>
       <c r="E41" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/TOI-2154b_2281_2023-11-20_Altair1999_1589_Lum</t>
+          <t>https://www.exoclock.space/database/observations/EPIC246851721b_1411_2023-11-20_Altair1999_1568_Clear</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>EPIC246851721b</t>
+          <t>TOI-2154b</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -1558,12 +1558,12 @@
       </c>
       <c r="D42" t="inlineStr">
         <is>
-          <t>NTHU TAT</t>
+          <t>NTHU Observatory</t>
         </is>
       </c>
       <c r="E42" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/EPIC246851721b_1411_2023-11-20_Altair1999_1568_Clear</t>
+          <t>https://www.exoclock.space/database/observations/TOI-2154b_2281_2023-11-20_Altair1999_1589_Lum</t>
         </is>
       </c>
     </row>
@@ -2164,7 +2164,7 @@
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>HAT-P-22b</t>
+          <t>GJ3470b</t>
         </is>
       </c>
       <c r="B65" t="inlineStr">
@@ -2174,24 +2174,24 @@
       </c>
       <c r="C65" t="inlineStr">
         <is>
-          <t>Hao-Yuan Duan</t>
+          <t>Kuo-Pin Huang</t>
         </is>
       </c>
       <c r="D65" t="inlineStr">
         <is>
-          <t>Lulin Observatory, Taiwan</t>
+          <t>Remote KMSH observatory</t>
         </is>
       </c>
       <c r="E65" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/HAT-P-22b_2749_2024-03-08_hyduan_2152_I</t>
+          <t>https://www.exoclock.space/database/observations/GJ3470b_2647_2024-03-08_kphuang_2112_R</t>
         </is>
       </c>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>GJ3470b</t>
+          <t>HAT-P-22b</t>
         </is>
       </c>
       <c r="B66" t="inlineStr">
@@ -2201,24 +2201,24 @@
       </c>
       <c r="C66" t="inlineStr">
         <is>
-          <t>Kuo-Pin Huang</t>
+          <t>Hao-Yuan Duan</t>
         </is>
       </c>
       <c r="D66" t="inlineStr">
         <is>
-          <t>Remote KMSH observatory</t>
+          <t>Lulin Observatory, Taiwan</t>
         </is>
       </c>
       <c r="E66" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/GJ3470b_2647_2024-03-08_kphuang_2112_R</t>
+          <t>https://www.exoclock.space/database/observations/HAT-P-22b_2749_2024-03-08_hyduan_2152_I</t>
         </is>
       </c>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>WASP-104b</t>
+          <t>HAT-P-36b</t>
         </is>
       </c>
       <c r="B67" t="inlineStr">
@@ -2228,17 +2228,17 @@
       </c>
       <c r="C67" t="inlineStr">
         <is>
-          <t>Hao-Yuan Duan</t>
+          <t>Yen-Hsing Lin</t>
         </is>
       </c>
       <c r="D67" t="inlineStr">
         <is>
-          <t>Lulin Observatory, Taiwan</t>
+          <t>NTHU TAT</t>
         </is>
       </c>
       <c r="E67" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/WASP-104b_5034_2024-03-12_hyduan_2152_I</t>
+          <t>https://www.exoclock.space/database/observations/HAT-P-36b_6657_2024-03-12_Altair1999_1568_R</t>
         </is>
       </c>
     </row>
@@ -2255,17 +2255,17 @@
       </c>
       <c r="C68" t="inlineStr">
         <is>
-          <t>YingLin Chen</t>
+          <t>Hao-Yuan Duan</t>
         </is>
       </c>
       <c r="D68" t="inlineStr">
         <is>
-          <t>CYGSH_Obseratory</t>
+          <t>Lulin Observatory, Taiwan</t>
         </is>
       </c>
       <c r="E68" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/WASP-104b_5034_2024-03-12_fredchen0930_1670_Clear</t>
+          <t>https://www.exoclock.space/database/observations/WASP-104b_5034_2024-03-12_hyduan_2152_I</t>
         </is>
       </c>
     </row>
@@ -2282,24 +2282,24 @@
       </c>
       <c r="C69" t="inlineStr">
         <is>
-          <t>Lee YuHsien</t>
+          <t>YingLin Chen</t>
         </is>
       </c>
       <c r="D69" t="inlineStr">
         <is>
-          <t>KMSH Observatory</t>
+          <t>CYGSH_Obseratory</t>
         </is>
       </c>
       <c r="E69" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/WASP-104b_5034_2024-03-12_KMSHO_1635_R</t>
+          <t>https://www.exoclock.space/database/observations/WASP-104b_5034_2024-03-12_fredchen0930_1670_Clear</t>
         </is>
       </c>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>HAT-P-36b</t>
+          <t>WASP-104b</t>
         </is>
       </c>
       <c r="B70" t="inlineStr">
@@ -2309,24 +2309,24 @@
       </c>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Yen-Hsing Lin</t>
+          <t>Lee YuHsien</t>
         </is>
       </c>
       <c r="D70" t="inlineStr">
         <is>
-          <t>NTHU TAT</t>
+          <t>KMSH Observatory</t>
         </is>
       </c>
       <c r="E70" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/HAT-P-36b_6657_2024-03-12_Altair1999_1568_R</t>
+          <t>https://www.exoclock.space/database/observations/WASP-104b_5034_2024-03-12_KMSHO_1635_R</t>
         </is>
       </c>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>WASP-104b</t>
+          <t>HAT-P-30b</t>
         </is>
       </c>
       <c r="B71" t="inlineStr">
@@ -2336,24 +2336,24 @@
       </c>
       <c r="C71" t="inlineStr">
         <is>
-          <t>Lee YuHsien</t>
+          <t>Ting-Shuo Yeh</t>
         </is>
       </c>
       <c r="D71" t="inlineStr">
         <is>
-          <t>KMSH Observatory</t>
+          <t>TCFSH Observatory</t>
         </is>
       </c>
       <c r="E71" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/WASP-104b_5038_2024-03-19_KMSHO_1635_R</t>
+          <t>https://www.exoclock.space/database/observations/HAT-P-30b_3146_2024-03-19_TCFSH_Obs_1371_R</t>
         </is>
       </c>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>HAT-P-30b</t>
+          <t>WASP-104b</t>
         </is>
       </c>
       <c r="B72" t="inlineStr">
@@ -2363,17 +2363,17 @@
       </c>
       <c r="C72" t="inlineStr">
         <is>
-          <t>Ting-Shuo Yeh</t>
+          <t>Lee YuHsien</t>
         </is>
       </c>
       <c r="D72" t="inlineStr">
         <is>
-          <t>TCFSH Observatory</t>
+          <t>KMSH Observatory</t>
         </is>
       </c>
       <c r="E72" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/HAT-P-30b_3146_2024-03-19_TCFSH_Obs_1371_R</t>
+          <t>https://www.exoclock.space/database/observations/WASP-104b_5038_2024-03-19_KMSHO_1635_R</t>
         </is>
       </c>
     </row>
@@ -2476,12 +2476,12 @@
       </c>
       <c r="D76" t="inlineStr">
         <is>
-          <t>NTHU Observatory</t>
+          <t>NTHU TAT</t>
         </is>
       </c>
       <c r="E76" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/Qatar-6b_2526_2024-04-02_Altair1999_1323_Lum</t>
+          <t>https://www.exoclock.space/database/observations/Qatar-6b_2526_2024-04-02_Altair1999_1568_R</t>
         </is>
       </c>
     </row>
@@ -2503,12 +2503,12 @@
       </c>
       <c r="D77" t="inlineStr">
         <is>
-          <t>NTHU TAT</t>
+          <t>NTHU Observatory</t>
         </is>
       </c>
       <c r="E77" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/Qatar-6b_2526_2024-04-02_Altair1999_1568_R</t>
+          <t>https://www.exoclock.space/database/observations/Qatar-6b_2526_2024-04-02_Altair1999_1323_Lum</t>
         </is>
       </c>
     </row>
@@ -3595,7 +3595,7 @@
     <row r="118">
       <c r="A118" t="inlineStr">
         <is>
-          <t>HAT-P-16b</t>
+          <t>WASP-33b</t>
         </is>
       </c>
       <c r="B118" t="inlineStr">
@@ -3605,24 +3605,24 @@
       </c>
       <c r="C118" t="inlineStr">
         <is>
-          <t>Lee YuHsien</t>
+          <t>Shun-Chia Yang</t>
         </is>
       </c>
       <c r="D118" t="inlineStr">
         <is>
-          <t>KMSH Observatory</t>
+          <t>Starry House Observatory</t>
         </is>
       </c>
       <c r="E118" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/HAT-P-16b_3269_2024-11-06_KMSHO_1635_R</t>
+          <t>https://www.exoclock.space/database/observations/WASP-33b_7440_2024-11-06_scyang_2506_R</t>
         </is>
       </c>
     </row>
     <row r="119">
       <c r="A119" t="inlineStr">
         <is>
-          <t>WASP-33b</t>
+          <t>HAT-P-16b</t>
         </is>
       </c>
       <c r="B119" t="inlineStr">
@@ -3632,17 +3632,17 @@
       </c>
       <c r="C119" t="inlineStr">
         <is>
-          <t>Shun-Chia Yang</t>
+          <t>Lee YuHsien</t>
         </is>
       </c>
       <c r="D119" t="inlineStr">
         <is>
-          <t>Starry House Observatory</t>
+          <t>KMSH Observatory</t>
         </is>
       </c>
       <c r="E119" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/WASP-33b_7440_2024-11-06_scyang_2506_R</t>
+          <t>https://www.exoclock.space/database/observations/HAT-P-16b_3269_2024-11-06_KMSHO_1635_R</t>
         </is>
       </c>
     </row>
@@ -3703,7 +3703,7 @@
     <row r="122">
       <c r="A122" t="inlineStr">
         <is>
-          <t>HAT-P-33b</t>
+          <t>GPX-1b</t>
         </is>
       </c>
       <c r="B122" t="inlineStr">
@@ -3713,17 +3713,17 @@
       </c>
       <c r="C122" t="inlineStr">
         <is>
-          <t>Yen-Hsing Lin</t>
+          <t>Lee YuHsien</t>
         </is>
       </c>
       <c r="D122" t="inlineStr">
         <is>
-          <t>Starry House Observatory</t>
+          <t>KMSH Observatory</t>
         </is>
       </c>
       <c r="E122" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/HAT-P-33b_2618_2024-11-27_Altair1999_2435_Lum</t>
+          <t>https://www.exoclock.space/database/observations/GPX-1b_5214_2024-11-27_KMSHO_1635_R</t>
         </is>
       </c>
     </row>
@@ -3757,7 +3757,7 @@
     <row r="124">
       <c r="A124" t="inlineStr">
         <is>
-          <t>GPX-1b</t>
+          <t>HAT-P-33b</t>
         </is>
       </c>
       <c r="B124" t="inlineStr">
@@ -3767,24 +3767,24 @@
       </c>
       <c r="C124" t="inlineStr">
         <is>
-          <t>Lee YuHsien</t>
+          <t>Yen-Hsing Lin</t>
         </is>
       </c>
       <c r="D124" t="inlineStr">
         <is>
-          <t>KMSH Observatory</t>
+          <t>Starry House Observatory</t>
         </is>
       </c>
       <c r="E124" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/GPX-1b_5214_2024-11-27_KMSHO_1635_R</t>
+          <t>https://www.exoclock.space/database/observations/HAT-P-33b_2618_2024-11-27_Altair1999_2435_Lum</t>
         </is>
       </c>
     </row>
     <row r="125">
       <c r="A125" t="inlineStr">
         <is>
-          <t>K2-34b</t>
+          <t>WASP-33b</t>
         </is>
       </c>
       <c r="B125" t="inlineStr">
@@ -3794,29 +3794,29 @@
       </c>
       <c r="C125" t="inlineStr">
         <is>
-          <t>Yen-Hsing Lin</t>
+          <t>Ting-Shuo Yeh</t>
         </is>
       </c>
       <c r="D125" t="inlineStr">
         <is>
-          <t>Starry House Observatory</t>
+          <t>TCFSH Observatory</t>
         </is>
       </c>
       <c r="E125" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/K2-34b_3037_2024-11-28_Altair1999_2435_Lum</t>
+          <t>https://www.exoclock.space/database/observations/WASP-33b_7458_2024-11-28_TCFSH_Obs_1371_R</t>
         </is>
       </c>
     </row>
     <row r="126">
       <c r="A126" t="inlineStr">
         <is>
-          <t>TOI-3714b</t>
+          <t>K2-34b</t>
         </is>
       </c>
       <c r="B126" t="inlineStr">
         <is>
-          <t>2024-11-29</t>
+          <t>2024-11-28</t>
         </is>
       </c>
       <c r="C126" t="inlineStr">
@@ -3831,7 +3831,7 @@
       </c>
       <c r="E126" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/TOI-3714b_4222_2024-11-29_Altair1999_2435_Lum</t>
+          <t>https://www.exoclock.space/database/observations/K2-34b_3037_2024-11-28_Altair1999_2435_Lum</t>
         </is>
       </c>
     </row>
@@ -3865,12 +3865,12 @@
     <row r="128">
       <c r="A128" t="inlineStr">
         <is>
-          <t>HAT-P-25b</t>
+          <t>TOI-3714b</t>
         </is>
       </c>
       <c r="B128" t="inlineStr">
         <is>
-          <t>2024-11-30</t>
+          <t>2024-11-29</t>
         </is>
       </c>
       <c r="C128" t="inlineStr">
@@ -3885,41 +3885,41 @@
       </c>
       <c r="E128" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/HAT-P-25b_2491_2024-11-30_Altair1999_2435_Lum</t>
+          <t>https://www.exoclock.space/database/observations/TOI-3714b_4222_2024-11-29_Altair1999_2435_Lum</t>
         </is>
       </c>
     </row>
     <row r="129">
       <c r="A129" t="inlineStr">
         <is>
-          <t>HAT-P-52b</t>
+          <t>HAT-P-25b</t>
         </is>
       </c>
       <c r="B129" t="inlineStr">
         <is>
-          <t>2024-12-01</t>
+          <t>2024-11-30</t>
         </is>
       </c>
       <c r="C129" t="inlineStr">
         <is>
-          <t>Lee YuHsien</t>
+          <t>Yen-Hsing Lin</t>
         </is>
       </c>
       <c r="D129" t="inlineStr">
         <is>
-          <t>KMSH Observatory</t>
+          <t>Starry House Observatory</t>
         </is>
       </c>
       <c r="E129" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/HAT-P-52b_3305_2024-12-01_KMSHO_1635_R</t>
+          <t>https://www.exoclock.space/database/observations/HAT-P-25b_2491_2024-11-30_Altair1999_2435_Lum</t>
         </is>
       </c>
     </row>
     <row r="130">
       <c r="A130" t="inlineStr">
         <is>
-          <t>TOI-3714b</t>
+          <t>HAT-P-52b</t>
         </is>
       </c>
       <c r="B130" t="inlineStr">
@@ -3939,19 +3939,19 @@
       </c>
       <c r="E130" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/TOI-3714b_4223_2024-12-01_KMSHO_1635_R</t>
+          <t>https://www.exoclock.space/database/observations/HAT-P-52b_3305_2024-12-01_KMSHO_1635_R</t>
         </is>
       </c>
     </row>
     <row r="131">
       <c r="A131" t="inlineStr">
         <is>
-          <t>K2-29b</t>
+          <t>TOI-3714b</t>
         </is>
       </c>
       <c r="B131" t="inlineStr">
         <is>
-          <t>2024-12-04</t>
+          <t>2024-12-01</t>
         </is>
       </c>
       <c r="C131" t="inlineStr">
@@ -3966,46 +3966,46 @@
       </c>
       <c r="E131" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/K2-29b_2793_2024-12-04_KMSHO_1635_R</t>
+          <t>https://www.exoclock.space/database/observations/TOI-3714b_4223_2024-12-01_KMSHO_1635_R</t>
         </is>
       </c>
     </row>
     <row r="132">
       <c r="A132" t="inlineStr">
         <is>
-          <t>Gaia-1b</t>
+          <t>K2-29b</t>
         </is>
       </c>
       <c r="B132" t="inlineStr">
         <is>
-          <t>2024-12-06</t>
+          <t>2024-12-04</t>
         </is>
       </c>
       <c r="C132" t="inlineStr">
         <is>
-          <t>Yen-Hsing Lin</t>
+          <t>Lee YuHsien</t>
         </is>
       </c>
       <c r="D132" t="inlineStr">
         <is>
-          <t>Starry House Observatory</t>
+          <t>KMSH Observatory</t>
         </is>
       </c>
       <c r="E132" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/Gaia-1b_2983_2024-12-06_Altair1999_2435_Lum</t>
+          <t>https://www.exoclock.space/database/observations/K2-29b_2793_2024-12-04_KMSHO_1635_R</t>
         </is>
       </c>
     </row>
     <row r="133">
       <c r="A133" t="inlineStr">
         <is>
-          <t>K2-121b</t>
+          <t>Gaia-1b</t>
         </is>
       </c>
       <c r="B133" t="inlineStr">
         <is>
-          <t>2024-12-09</t>
+          <t>2024-12-06</t>
         </is>
       </c>
       <c r="C133" t="inlineStr">
@@ -4020,46 +4020,46 @@
       </c>
       <c r="E133" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/K2-121b_1756_2024-12-09_Altair1999_2435_Lum</t>
+          <t>https://www.exoclock.space/database/observations/Gaia-1b_2983_2024-12-06_Altair1999_2435_Lum</t>
         </is>
       </c>
     </row>
     <row r="134">
       <c r="A134" t="inlineStr">
         <is>
-          <t>XO-2Nb</t>
+          <t>K2-121b</t>
         </is>
       </c>
       <c r="B134" t="inlineStr">
         <is>
-          <t>2024-12-16</t>
+          <t>2024-12-09</t>
         </is>
       </c>
       <c r="C134" t="inlineStr">
         <is>
-          <t>Lee YuHsien</t>
+          <t>Yen-Hsing Lin</t>
         </is>
       </c>
       <c r="D134" t="inlineStr">
         <is>
-          <t>KMSH Observatory</t>
+          <t>Starry House Observatory</t>
         </is>
       </c>
       <c r="E134" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/XO-2Nb_3484_2024-12-16_KMSHO_1635_R</t>
+          <t>https://www.exoclock.space/database/observations/K2-121b_1756_2024-12-09_Altair1999_2435_Lum</t>
         </is>
       </c>
     </row>
     <row r="135">
       <c r="A135" t="inlineStr">
         <is>
-          <t>WASP-43b</t>
+          <t>XO-2Nb</t>
         </is>
       </c>
       <c r="B135" t="inlineStr">
         <is>
-          <t>2024-12-19</t>
+          <t>2024-12-16</t>
         </is>
       </c>
       <c r="C135" t="inlineStr">
@@ -4074,7 +4074,7 @@
       </c>
       <c r="E135" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/WASP-43b_11210_2024-12-19_KMSHO_1635_R</t>
+          <t>https://www.exoclock.space/database/observations/XO-2Nb_3484_2024-12-16_KMSHO_1635_R</t>
         </is>
       </c>
     </row>
@@ -4108,12 +4108,12 @@
     <row r="137">
       <c r="A137" t="inlineStr">
         <is>
-          <t>KELT-19Ab</t>
+          <t>WASP-43b</t>
         </is>
       </c>
       <c r="B137" t="inlineStr">
         <is>
-          <t>2024-12-21</t>
+          <t>2024-12-19</t>
         </is>
       </c>
       <c r="C137" t="inlineStr">
@@ -4128,19 +4128,19 @@
       </c>
       <c r="E137" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/KELT-19Ab_1977_2024-12-21_KMSHO_1635_R</t>
+          <t>https://www.exoclock.space/database/observations/WASP-43b_11210_2024-12-19_KMSHO_1635_R</t>
         </is>
       </c>
     </row>
     <row r="138">
       <c r="A138" t="inlineStr">
         <is>
-          <t>K2-34b</t>
+          <t>KELT-7b</t>
         </is>
       </c>
       <c r="B138" t="inlineStr">
         <is>
-          <t>2024-12-28</t>
+          <t>2024-12-20</t>
         </is>
       </c>
       <c r="C138" t="inlineStr">
@@ -4155,73 +4155,73 @@
       </c>
       <c r="E138" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/K2-34b_3047_2024-12-28_KMSHO_1635_R</t>
+          <t>https://www.exoclock.space/database/observations/KELT-7b_3334_2024-12-20_KMSHO_1635_R</t>
         </is>
       </c>
     </row>
     <row r="139">
       <c r="A139" t="inlineStr">
         <is>
-          <t>HAT-P-42b</t>
+          <t>KELT-19Ab</t>
         </is>
       </c>
       <c r="B139" t="inlineStr">
         <is>
-          <t>2024-12-28</t>
+          <t>2024-12-21</t>
         </is>
       </c>
       <c r="C139" t="inlineStr">
         <is>
-          <t>Yen-Hsing Lin</t>
+          <t>Lee YuHsien</t>
         </is>
       </c>
       <c r="D139" t="inlineStr">
         <is>
-          <t>Starry House Observatory</t>
+          <t>KMSH Observatory</t>
         </is>
       </c>
       <c r="E139" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/HAT-P-42b_1966_2024-12-28_Altair1999_2435_Lum</t>
+          <t>https://www.exoclock.space/database/observations/KELT-19Ab_1977_2024-12-21_KMSHO_1635_R</t>
         </is>
       </c>
     </row>
     <row r="140">
       <c r="A140" t="inlineStr">
         <is>
-          <t>WASP-85Ab</t>
+          <t>K2-34b</t>
         </is>
       </c>
       <c r="B140" t="inlineStr">
         <is>
-          <t>2024-12-29</t>
+          <t>2024-12-28</t>
         </is>
       </c>
       <c r="C140" t="inlineStr">
         <is>
-          <t>Yen-Hsing Lin</t>
+          <t>Lee YuHsien</t>
         </is>
       </c>
       <c r="D140" t="inlineStr">
         <is>
-          <t>Starry House Observatory</t>
+          <t>KMSH Observatory</t>
         </is>
       </c>
       <c r="E140" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/WASP-85Ab_3437_2024-12-29_Altair1999_2435_Lum</t>
+          <t>https://www.exoclock.space/database/observations/K2-34b_3047_2024-12-28_KMSHO_1635_R</t>
         </is>
       </c>
     </row>
     <row r="141">
       <c r="A141" t="inlineStr">
         <is>
-          <t>TOI-2364b</t>
+          <t>HAT-P-42b</t>
         </is>
       </c>
       <c r="B141" t="inlineStr">
         <is>
-          <t>2024-12-29</t>
+          <t>2024-12-28</t>
         </is>
       </c>
       <c r="C141" t="inlineStr">
@@ -4236,46 +4236,46 @@
       </c>
       <c r="E141" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/TOI-2364b_2271_2024-12-29_Altair1999_2435_Lum</t>
+          <t>https://www.exoclock.space/database/observations/HAT-P-42b_1966_2024-12-28_Altair1999_2435_Lum</t>
         </is>
       </c>
     </row>
     <row r="142">
       <c r="A142" t="inlineStr">
         <is>
-          <t>TOI-628b</t>
+          <t>TOI-2364b</t>
         </is>
       </c>
       <c r="B142" t="inlineStr">
         <is>
-          <t>2024-12-30</t>
+          <t>2024-12-29</t>
         </is>
       </c>
       <c r="C142" t="inlineStr">
         <is>
-          <t>Lee YuHsien</t>
+          <t>Yen-Hsing Lin</t>
         </is>
       </c>
       <c r="D142" t="inlineStr">
         <is>
-          <t>KMSH Observatory</t>
+          <t>Starry House Observatory</t>
         </is>
       </c>
       <c r="E142" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/TOI-628b_2677_2024-12-30_KMSHO_1635_R</t>
+          <t>https://www.exoclock.space/database/observations/TOI-2364b_2271_2024-12-29_Altair1999_2435_Lum</t>
         </is>
       </c>
     </row>
     <row r="143">
       <c r="A143" t="inlineStr">
         <is>
-          <t>CoRoT-5b</t>
+          <t>WASP-85Ab</t>
         </is>
       </c>
       <c r="B143" t="inlineStr">
         <is>
-          <t>2024-12-30</t>
+          <t>2024-12-29</t>
         </is>
       </c>
       <c r="C143" t="inlineStr">
@@ -4290,46 +4290,46 @@
       </c>
       <c r="E143" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/CoRoT-5b_2261_2024-12-30_Altair1999_2435_Lum</t>
+          <t>https://www.exoclock.space/database/observations/WASP-85Ab_3437_2024-12-29_Altair1999_2435_Lum</t>
         </is>
       </c>
     </row>
     <row r="144">
       <c r="A144" t="inlineStr">
         <is>
-          <t>CoRoT-1b</t>
+          <t>CoRoT-5b</t>
         </is>
       </c>
       <c r="B144" t="inlineStr">
         <is>
-          <t>2025-01-02</t>
+          <t>2024-12-30</t>
         </is>
       </c>
       <c r="C144" t="inlineStr">
         <is>
-          <t>Lee YuHsien</t>
+          <t>Yen-Hsing Lin</t>
         </is>
       </c>
       <c r="D144" t="inlineStr">
         <is>
-          <t>KMSH Observatory</t>
+          <t>Starry House Observatory</t>
         </is>
       </c>
       <c r="E144" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/CoRoT-1b_6052_2025-01-02_KMSHO_1635_R</t>
+          <t>https://www.exoclock.space/database/observations/CoRoT-5b_2261_2024-12-30_Altair1999_2435_Lum</t>
         </is>
       </c>
     </row>
     <row r="145">
       <c r="A145" t="inlineStr">
         <is>
-          <t>K2-34b</t>
+          <t>TOI-628b</t>
         </is>
       </c>
       <c r="B145" t="inlineStr">
         <is>
-          <t>2025-01-03</t>
+          <t>2024-12-30</t>
         </is>
       </c>
       <c r="C145" t="inlineStr">
@@ -4344,19 +4344,19 @@
       </c>
       <c r="E145" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/K2-34b_3049_2025-01-03_KMSHO_1635_R</t>
+          <t>https://www.exoclock.space/database/observations/TOI-628b_2677_2024-12-30_KMSHO_1635_R</t>
         </is>
       </c>
     </row>
     <row r="146">
       <c r="A146" t="inlineStr">
         <is>
-          <t>XO-2Nb</t>
+          <t>CoRoT-1b</t>
         </is>
       </c>
       <c r="B146" t="inlineStr">
         <is>
-          <t>2025-01-06</t>
+          <t>2025-01-02</t>
         </is>
       </c>
       <c r="C146" t="inlineStr">
@@ -4371,19 +4371,19 @@
       </c>
       <c r="E146" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/XO-2Nb_3492_2025-01-06_KMSHO_1635_R</t>
+          <t>https://www.exoclock.space/database/observations/CoRoT-1b_6052_2025-01-02_KMSHO_1635_R</t>
         </is>
       </c>
     </row>
     <row r="147">
       <c r="A147" t="inlineStr">
         <is>
-          <t>WASP-104b</t>
+          <t>K2-34b</t>
         </is>
       </c>
       <c r="B147" t="inlineStr">
         <is>
-          <t>2025-01-06</t>
+          <t>2025-01-03</t>
         </is>
       </c>
       <c r="C147" t="inlineStr">
@@ -4398,14 +4398,14 @@
       </c>
       <c r="E147" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/WASP-104b_5205_2025-01-06_KMSHO_1635_R</t>
+          <t>https://www.exoclock.space/database/observations/K2-34b_3049_2025-01-03_KMSHO_1635_R</t>
         </is>
       </c>
     </row>
     <row r="148">
       <c r="A148" t="inlineStr">
         <is>
-          <t>K2-34b</t>
+          <t>WASP-104b</t>
         </is>
       </c>
       <c r="B148" t="inlineStr">
@@ -4415,29 +4415,29 @@
       </c>
       <c r="C148" t="inlineStr">
         <is>
-          <t>Yen-Hsing Lin</t>
+          <t>Lee YuHsien</t>
         </is>
       </c>
       <c r="D148" t="inlineStr">
         <is>
-          <t>Starry House Observatory</t>
+          <t>KMSH Observatory</t>
         </is>
       </c>
       <c r="E148" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/K2-34b_3050_2025-01-06_Altair1999_2435_Lum</t>
+          <t>https://www.exoclock.space/database/observations/WASP-104b_5205_2025-01-06_KMSHO_1635_R</t>
         </is>
       </c>
     </row>
     <row r="149">
       <c r="A149" t="inlineStr">
         <is>
-          <t>GPX-1b</t>
+          <t>XO-2Nb</t>
         </is>
       </c>
       <c r="B149" t="inlineStr">
         <is>
-          <t>2025-01-08</t>
+          <t>2025-01-06</t>
         </is>
       </c>
       <c r="C149" t="inlineStr">
@@ -4452,46 +4452,46 @@
       </c>
       <c r="E149" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/GPX-1b_5238_2025-01-08_KMSHO_1635_R</t>
+          <t>https://www.exoclock.space/database/observations/XO-2Nb_3492_2025-01-06_KMSHO_1635_R</t>
         </is>
       </c>
     </row>
     <row r="150">
       <c r="A150" t="inlineStr">
         <is>
-          <t>WASP-84b</t>
+          <t>K2-34b</t>
         </is>
       </c>
       <c r="B150" t="inlineStr">
         <is>
-          <t>2025-01-08</t>
+          <t>2025-01-06</t>
         </is>
       </c>
       <c r="C150" t="inlineStr">
         <is>
-          <t>Lee YuHsien</t>
+          <t>Yen-Hsing Lin</t>
         </is>
       </c>
       <c r="D150" t="inlineStr">
         <is>
-          <t>KMSH Observatory</t>
+          <t>Starry House Observatory</t>
         </is>
       </c>
       <c r="E150" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/WASP-84b_1072_2025-01-08_KMSHO_1635_R</t>
+          <t>https://www.exoclock.space/database/observations/K2-34b_3050_2025-01-06_Altair1999_2435_Lum</t>
         </is>
       </c>
     </row>
     <row r="151">
       <c r="A151" t="inlineStr">
         <is>
-          <t>WASP-36b</t>
+          <t>GPX-1b</t>
         </is>
       </c>
       <c r="B151" t="inlineStr">
         <is>
-          <t>2025-01-10</t>
+          <t>2025-01-08</t>
         </is>
       </c>
       <c r="C151" t="inlineStr">
@@ -4506,19 +4506,19 @@
       </c>
       <c r="E151" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/WASP-36b_5946_2025-01-10_KMSHO_1635_R</t>
+          <t>https://www.exoclock.space/database/observations/GPX-1b_5238_2025-01-08_KMSHO_1635_R</t>
         </is>
       </c>
     </row>
     <row r="152">
       <c r="A152" t="inlineStr">
         <is>
-          <t>WASP-43b</t>
+          <t>WASP-84b</t>
         </is>
       </c>
       <c r="B152" t="inlineStr">
         <is>
-          <t>2025-01-10</t>
+          <t>2025-01-08</t>
         </is>
       </c>
       <c r="C152" t="inlineStr">
@@ -4533,19 +4533,19 @@
       </c>
       <c r="E152" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/WASP-43b_11237_2025-01-10_KMSHO_1635_R</t>
+          <t>https://www.exoclock.space/database/observations/WASP-84b_1072_2025-01-08_KMSHO_1635_R</t>
         </is>
       </c>
     </row>
     <row r="153">
       <c r="A153" t="inlineStr">
         <is>
-          <t>K2-34b</t>
+          <t>WASP-43b</t>
         </is>
       </c>
       <c r="B153" t="inlineStr">
         <is>
-          <t>2025-01-12</t>
+          <t>2025-01-10</t>
         </is>
       </c>
       <c r="C153" t="inlineStr">
@@ -4560,41 +4560,41 @@
       </c>
       <c r="E153" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/K2-34b_3052_2025-01-12_KMSHO_1635_R</t>
+          <t>https://www.exoclock.space/database/observations/WASP-43b_11237_2025-01-10_KMSHO_1635_R</t>
         </is>
       </c>
     </row>
     <row r="154">
       <c r="A154" t="inlineStr">
         <is>
-          <t>HAT-P-13b</t>
+          <t>WASP-36b</t>
         </is>
       </c>
       <c r="B154" t="inlineStr">
         <is>
-          <t>2025-01-12</t>
+          <t>2025-01-10</t>
         </is>
       </c>
       <c r="C154" t="inlineStr">
         <is>
-          <t>Yen-Hsing Lin</t>
+          <t>Lee YuHsien</t>
         </is>
       </c>
       <c r="D154" t="inlineStr">
         <is>
-          <t>Starry House Observatory</t>
+          <t>KMSH Observatory</t>
         </is>
       </c>
       <c r="E154" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/HAT-P-13b_3135_2025-01-12_Altair1999_2435_Lum</t>
+          <t>https://www.exoclock.space/database/observations/WASP-36b_5946_2025-01-10_KMSHO_1635_R</t>
         </is>
       </c>
     </row>
     <row r="155">
       <c r="A155" t="inlineStr">
         <is>
-          <t>K2-405b</t>
+          <t>HAT-P-13b</t>
         </is>
       </c>
       <c r="B155" t="inlineStr">
@@ -4609,105 +4609,105 @@
       </c>
       <c r="D155" t="inlineStr">
         <is>
-          <t>Lulin Observatory</t>
+          <t>Starry House Observatory</t>
         </is>
       </c>
       <c r="E155" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/K2-405b_2661_2025-01-12_Altair1999_2155_R</t>
+          <t>https://www.exoclock.space/database/observations/HAT-P-13b_3135_2025-01-12_Altair1999_2435_Lum</t>
         </is>
       </c>
     </row>
     <row r="156">
       <c r="A156" t="inlineStr">
         <is>
-          <t>WASP-104b</t>
+          <t>K2-34b</t>
         </is>
       </c>
       <c r="B156" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-12</t>
         </is>
       </c>
       <c r="C156" t="inlineStr">
         <is>
-          <t>Yen-Hsing Lin</t>
+          <t>Lee YuHsien</t>
         </is>
       </c>
       <c r="D156" t="inlineStr">
         <is>
-          <t>Starry House Observatory</t>
+          <t>KMSH Observatory</t>
         </is>
       </c>
       <c r="E156" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/WASP-104b_5209_2025-01-13_Altair1999_2606_R</t>
+          <t>https://www.exoclock.space/database/observations/K2-34b_3052_2025-01-12_KMSHO_1635_R</t>
         </is>
       </c>
     </row>
     <row r="157">
       <c r="A157" t="inlineStr">
         <is>
-          <t>WASP-36b</t>
+          <t>K2-405b</t>
         </is>
       </c>
       <c r="B157" t="inlineStr">
         <is>
-          <t>2025-01-13</t>
+          <t>2025-01-12</t>
         </is>
       </c>
       <c r="C157" t="inlineStr">
         <is>
-          <t>Lee YuHsien</t>
+          <t>Yen-Hsing Lin</t>
         </is>
       </c>
       <c r="D157" t="inlineStr">
         <is>
-          <t>KMSH Observatory</t>
+          <t>Lulin Observatory</t>
         </is>
       </c>
       <c r="E157" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/WASP-36b_5948_2025-01-13_KMSHO_1635_R</t>
+          <t>https://www.exoclock.space/database/observations/K2-405b_2661_2025-01-12_Altair1999_2155_R</t>
         </is>
       </c>
     </row>
     <row r="158">
       <c r="A158" t="inlineStr">
         <is>
-          <t>NGTS-9b</t>
+          <t>WASP-36b</t>
         </is>
       </c>
       <c r="B158" t="inlineStr">
         <is>
-          <t>2025-01-16</t>
+          <t>2025-01-13</t>
         </is>
       </c>
       <c r="C158" t="inlineStr">
         <is>
-          <t>Yen-Hsing Lin</t>
+          <t>Lee YuHsien</t>
         </is>
       </c>
       <c r="D158" t="inlineStr">
         <is>
-          <t>Lulin Observatory</t>
+          <t>KMSH Observatory</t>
         </is>
       </c>
       <c r="E158" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/NGTS-9b_2062_2025-01-16_Altair1999_2155_R</t>
+          <t>https://www.exoclock.space/database/observations/WASP-36b_5948_2025-01-13_KMSHO_1635_R</t>
         </is>
       </c>
     </row>
     <row r="159">
       <c r="A159" t="inlineStr">
         <is>
-          <t>WASP-34b</t>
+          <t>WASP-104b</t>
         </is>
       </c>
       <c r="B159" t="inlineStr">
         <is>
-          <t>2025-01-16</t>
+          <t>2025-01-13</t>
         </is>
       </c>
       <c r="C159" t="inlineStr">
@@ -4722,14 +4722,14 @@
       </c>
       <c r="E159" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/WASP-34b_2118_2025-01-16_Altair1999_2606_R</t>
+          <t>https://www.exoclock.space/database/observations/WASP-104b_5209_2025-01-13_Altair1999_2606_R</t>
         </is>
       </c>
     </row>
     <row r="160">
       <c r="A160" t="inlineStr">
         <is>
-          <t>HAT-P-21b</t>
+          <t>WASP-34b</t>
         </is>
       </c>
       <c r="B160" t="inlineStr">
@@ -4739,44 +4739,260 @@
       </c>
       <c r="C160" t="inlineStr">
         <is>
-          <t>Lee YuHsien</t>
+          <t>Yen-Hsing Lin</t>
         </is>
       </c>
       <c r="D160" t="inlineStr">
         <is>
-          <t>KMSH Observatory</t>
+          <t>Starry House Observatory</t>
         </is>
       </c>
       <c r="E160" t="inlineStr">
         <is>
-          <t>https://www.exoclock.space/database/observations/HAT-P-21b_2217_2025-01-16_KMSHO_1635_R</t>
+          <t>https://www.exoclock.space/database/observations/WASP-34b_2118_2025-01-16_Altair1999_2606_R</t>
         </is>
       </c>
     </row>
     <row r="161">
       <c r="A161" t="inlineStr">
         <is>
+          <t>NGTS-9b</t>
+        </is>
+      </c>
+      <c r="B161" t="inlineStr">
+        <is>
+          <t>2025-01-16</t>
+        </is>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>Yen-Hsing Lin</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>Lulin Observatory</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>https://www.exoclock.space/database/observations/NGTS-9b_2062_2025-01-16_Altair1999_2155_R</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="inlineStr">
+        <is>
+          <t>HAT-P-21b</t>
+        </is>
+      </c>
+      <c r="B162" t="inlineStr">
+        <is>
+          <t>2025-01-16</t>
+        </is>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>Lee YuHsien</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>KMSH Observatory</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>https://www.exoclock.space/database/observations/HAT-P-21b_2217_2025-01-16_KMSHO_1635_R</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="inlineStr">
+        <is>
           <t>TOI-1811b</t>
         </is>
       </c>
-      <c r="B161" t="inlineStr">
+      <c r="B163" t="inlineStr">
         <is>
           <t>2025-01-17</t>
         </is>
       </c>
-      <c r="C161" t="inlineStr">
+      <c r="C163" t="inlineStr">
         <is>
           <t>Lee YuHsien</t>
         </is>
       </c>
-      <c r="D161" t="inlineStr">
+      <c r="D163" t="inlineStr">
         <is>
           <t>KMSH Observatory</t>
         </is>
       </c>
-      <c r="E161" t="inlineStr">
+      <c r="E163" t="inlineStr">
         <is>
           <t>https://www.exoclock.space/database/observations/TOI-1811b_2463_2025-01-17_KMSHO_1635_R</t>
+        </is>
+      </c>
+    </row>
+    <row r="164">
+      <c r="A164" t="inlineStr">
+        <is>
+          <t>KPS-1b</t>
+        </is>
+      </c>
+      <c r="B164" t="inlineStr">
+        <is>
+          <t>2025-02-09</t>
+        </is>
+      </c>
+      <c r="C164" t="inlineStr">
+        <is>
+          <t>Yen-Hsing Lin</t>
+        </is>
+      </c>
+      <c r="D164" t="inlineStr">
+        <is>
+          <t>Starry House Observatory</t>
+        </is>
+      </c>
+      <c r="E164" t="inlineStr">
+        <is>
+          <t>https://www.exoclock.space/database/observations/KPS-1b_5374_2025-02-09_Altair1999_2435_Lum</t>
+        </is>
+      </c>
+    </row>
+    <row r="165">
+      <c r="A165" t="inlineStr">
+        <is>
+          <t>K2-34b</t>
+        </is>
+      </c>
+      <c r="B165" t="inlineStr">
+        <is>
+          <t>2025-02-14</t>
+        </is>
+      </c>
+      <c r="C165" t="inlineStr">
+        <is>
+          <t>Yen-Hsing Lin</t>
+        </is>
+      </c>
+      <c r="D165" t="inlineStr">
+        <is>
+          <t>Starry House Observatory</t>
+        </is>
+      </c>
+      <c r="E165" t="inlineStr">
+        <is>
+          <t>https://www.exoclock.space/database/observations/K2-34b_3063_2025-02-14_Altair1999_2435_Lum</t>
+        </is>
+      </c>
+    </row>
+    <row r="166">
+      <c r="A166" t="inlineStr">
+        <is>
+          <t>TOI-532b</t>
+        </is>
+      </c>
+      <c r="B166" t="inlineStr">
+        <is>
+          <t>2025-02-18</t>
+        </is>
+      </c>
+      <c r="C166" t="inlineStr">
+        <is>
+          <t>Yen-Hsing Lin</t>
+        </is>
+      </c>
+      <c r="D166" t="inlineStr">
+        <is>
+          <t>Lulin Observatory</t>
+        </is>
+      </c>
+      <c r="E166" t="inlineStr">
+        <is>
+          <t>https://www.exoclock.space/database/observations/TOI-532b_3945_2025-02-18_Altair1999_2155_R</t>
+        </is>
+      </c>
+    </row>
+    <row r="167">
+      <c r="A167" t="inlineStr">
+        <is>
+          <t>K2-19b</t>
+        </is>
+      </c>
+      <c r="B167" t="inlineStr">
+        <is>
+          <t>2025-02-19</t>
+        </is>
+      </c>
+      <c r="C167" t="inlineStr">
+        <is>
+          <t>Yen-Hsing Lin</t>
+        </is>
+      </c>
+      <c r="D167" t="inlineStr">
+        <is>
+          <t>Lulin Observatory</t>
+        </is>
+      </c>
+      <c r="E167" t="inlineStr">
+        <is>
+          <t>https://www.exoclock.space/database/observations/K2-19b_1159_2025-02-19_Altair1999_2155_R</t>
+        </is>
+      </c>
+    </row>
+    <row r="168">
+      <c r="A168" t="inlineStr">
+        <is>
+          <t>WASP-36b</t>
+        </is>
+      </c>
+      <c r="B168" t="inlineStr">
+        <is>
+          <t>2025-03-08</t>
+        </is>
+      </c>
+      <c r="C168" t="inlineStr">
+        <is>
+          <t>Yen-Hsing Lin</t>
+        </is>
+      </c>
+      <c r="D168" t="inlineStr">
+        <is>
+          <t>Starry House Observatory</t>
+        </is>
+      </c>
+      <c r="E168" t="inlineStr">
+        <is>
+          <t>https://www.exoclock.space/database/observations/WASP-36b_5983_2025-03-08_Altair1999_2435_Lum</t>
+        </is>
+      </c>
+    </row>
+    <row r="169">
+      <c r="A169" t="inlineStr">
+        <is>
+          <t>Qatar-6b</t>
+        </is>
+      </c>
+      <c r="B169" t="inlineStr">
+        <is>
+          <t>2025-03-08</t>
+        </is>
+      </c>
+      <c r="C169" t="inlineStr">
+        <is>
+          <t>Yen-Hsing Lin</t>
+        </is>
+      </c>
+      <c r="D169" t="inlineStr">
+        <is>
+          <t>Starry House Observatory</t>
+        </is>
+      </c>
+      <c r="E169" t="inlineStr">
+        <is>
+          <t>https://www.exoclock.space/database/observations/Qatar-6b_2623_2025-03-08_Altair1999_2435_Lum</t>
         </is>
       </c>
     </row>

</xml_diff>